<commit_message>
added menu test file
</commit_message>
<xml_diff>
--- a/dataframe.xlsx
+++ b/dataframe.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -888,6 +888,14 @@
         <v>9781449357016</v>
       </c>
     </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2">
+        <v>64</v>
+      </c>
+      <c r="B64" s="1">
+        <v>9781492087830</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added menu, added pickle script to persist data
</commit_message>
<xml_diff>
--- a/dataframe.xlsx
+++ b/dataframe.xlsx
@@ -890,10 +890,10 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>9781492087830</v>
+        <v>9780471164838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>